<commit_message>
rewrite Iteration4 Using extends
</commit_message>
<xml_diff>
--- a/Assignment1-guess-number/Iteration4/document/time_log.xlsx
+++ b/Assignment1-guess-number/Iteration4/document/time_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shukebeta/OneDrive - Ara Institute of Canterbury/BCPR280/Assignment1-guess-number/Iteration2/document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shukebeta/OneDrive - Ara Institute of Canterbury/BCPR280/Assignment1-guess-number/Iteration4/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{9B27C467-49CD-DB42-B39F-B8AE1ACF5BEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2A7AFE8F-187C-0E40-B442-B954FC59FD60}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{9B27C467-49CD-DB42-B39F-B8AE1ACF5BEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{861DA568-F784-5E4A-B48F-E35AC7E5FCD4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
     <t>Amitrajit Sarkar</t>
   </si>
   <si>
-    <t>BCPR280-Iteration2</t>
+    <t>BCPR280-Iteration4</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1064,16 +1064,16 @@
         <v>37</v>
       </c>
       <c r="C7" s="15">
-        <v>43555</v>
+        <v>43563</v>
       </c>
       <c r="D7" s="16">
-        <v>0.41666666666666669</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F7" s="16">
-        <v>0.42708333333333331</v>
+        <v>0.6875</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1081,16 +1081,16 @@
         <v>38</v>
       </c>
       <c r="C8" s="15">
-        <v>43555</v>
+        <v>43563</v>
       </c>
       <c r="D8" s="16">
-        <v>0.43055555555555558</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="F8" s="16">
-        <v>0.4375</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="G8">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1098,16 +1098,16 @@
         <v>39</v>
       </c>
       <c r="C9" s="15">
-        <v>43555</v>
+        <v>43563</v>
       </c>
       <c r="D9" s="16">
-        <v>0.44097222222222227</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F9" s="16">
-        <v>0.44791666666666669</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1115,16 +1115,16 @@
         <v>40</v>
       </c>
       <c r="C10" s="15">
-        <v>43555</v>
+        <v>43563</v>
       </c>
       <c r="D10" s="16">
-        <v>0.45833333333333331</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="F10" s="16">
-        <v>0.46527777777777773</v>
+        <v>0.8125</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1132,16 +1132,16 @@
         <v>41</v>
       </c>
       <c r="C11" s="15">
-        <v>43555</v>
+        <v>43563</v>
       </c>
       <c r="D11" s="16">
-        <v>0.47222222222222227</v>
+        <v>0.8125</v>
       </c>
       <c r="F11" s="16">
-        <v>0.47916666666666669</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>